<commit_message>
Finish all tests with realistic values, check and fix ambience jaccard computation, check and tune fill degree of Bloom filters
</commit_message>
<xml_diff>
--- a/testlaeufe.xlsx
+++ b/testlaeufe.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>simQuery()</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Testlauf Nr.</t>
   </si>
   <si>
-    <t>d</t>
-  </si>
-  <si>
     <t>1, 3, 4</t>
   </si>
   <si>
@@ -67,6 +64,36 @@
   </si>
   <si>
     <t>2, 3, 6</t>
+  </si>
+  <si>
+    <t>3, 5, 10</t>
+  </si>
+  <si>
+    <t>4, 6, 7</t>
+  </si>
+  <si>
+    <t>2, 3, 5</t>
+  </si>
+  <si>
+    <t>1, 2, 6</t>
+  </si>
+  <si>
+    <t>1, 3, 2</t>
+  </si>
+  <si>
+    <t>3, 4, 6</t>
+  </si>
+  <si>
+    <t>1, 3, 7</t>
+  </si>
+  <si>
+    <t>3, 4, 5</t>
+  </si>
+  <si>
+    <t>1, 2, 7</t>
+  </si>
+  <si>
+    <t>2, 3, 4</t>
   </si>
 </sst>
 </file>
@@ -115,8 +142,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -133,19 +162,21 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -475,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -530,8 +561,8 @@
       <c r="C2">
         <v>100</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
+      <c r="D2">
+        <v>3</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -540,7 +571,7 @@
         <v>21</v>
       </c>
       <c r="I2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -553,8 +584,8 @@
       <c r="C3">
         <v>100</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
+      <c r="D3">
+        <v>3</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -563,7 +594,7 @@
         <v>14</v>
       </c>
       <c r="I3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -576,8 +607,8 @@
       <c r="C4">
         <v>100</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
+      <c r="D4">
+        <v>3</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -586,7 +617,7 @@
         <v>8</v>
       </c>
       <c r="I4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -599,8 +630,8 @@
       <c r="C5">
         <v>100</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
+      <c r="D5">
+        <v>3</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -609,7 +640,7 @@
         <v>47</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -622,8 +653,8 @@
       <c r="C6">
         <v>100</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
+      <c r="D6">
+        <v>3</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -632,7 +663,7 @@
         <v>96</v>
       </c>
       <c r="I6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -645,8 +676,8 @@
       <c r="C7">
         <v>100</v>
       </c>
-      <c r="D7" t="s">
-        <v>9</v>
+      <c r="D7">
+        <v>3</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -655,7 +686,7 @@
         <v>29</v>
       </c>
       <c r="I7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -668,17 +699,17 @@
       <c r="C8">
         <v>100</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>8</v>
+      </c>
+      <c r="I8" t="s">
         <v>9</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="H8">
-        <v>8</v>
-      </c>
-      <c r="I8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -691,8 +722,8 @@
       <c r="C9">
         <v>100</v>
       </c>
-      <c r="D9" t="s">
-        <v>9</v>
+      <c r="D9">
+        <v>3</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -701,7 +732,7 @@
         <v>48</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -714,17 +745,17 @@
       <c r="C10">
         <v>100</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
         <v>9</v>
-      </c>
-      <c r="E10">
-        <v>3</v>
-      </c>
-      <c r="H10">
-        <v>3</v>
-      </c>
-      <c r="I10" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -737,8 +768,8 @@
       <c r="C11">
         <v>100</v>
       </c>
-      <c r="D11" t="s">
-        <v>9</v>
+      <c r="D11">
+        <v>3</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -747,7 +778,7 @@
         <v>19</v>
       </c>
       <c r="I11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -760,8 +791,8 @@
       <c r="C12">
         <v>100</v>
       </c>
-      <c r="D12" t="s">
-        <v>9</v>
+      <c r="D12">
+        <v>3</v>
       </c>
       <c r="E12">
         <v>3</v>
@@ -770,7 +801,7 @@
         <v>9</v>
       </c>
       <c r="I12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -783,8 +814,8 @@
       <c r="C13">
         <v>100</v>
       </c>
-      <c r="D13" t="s">
-        <v>9</v>
+      <c r="D13">
+        <v>3</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -793,7 +824,631 @@
         <v>32</v>
       </c>
       <c r="I13" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>256</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>50</v>
+      </c>
+      <c r="H14">
+        <v>56</v>
+      </c>
+      <c r="I14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>256</v>
+      </c>
+      <c r="C15">
+        <v>100</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>21</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>256</v>
+      </c>
+      <c r="C16">
+        <v>100</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>50</v>
+      </c>
+      <c r="H16">
+        <v>44</v>
+      </c>
+      <c r="I16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>256</v>
+      </c>
+      <c r="C17">
+        <v>100</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>7</v>
+      </c>
+      <c r="H17">
+        <v>41</v>
+      </c>
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>256</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>50</v>
+      </c>
+      <c r="H18">
+        <v>57</v>
+      </c>
+      <c r="I18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>256</v>
+      </c>
+      <c r="C19">
+        <v>100</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>7</v>
+      </c>
+      <c r="H19">
+        <v>14</v>
+      </c>
+      <c r="I19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>256</v>
+      </c>
+      <c r="C20">
+        <v>100</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>50</v>
+      </c>
+      <c r="H20">
+        <v>6</v>
+      </c>
+      <c r="I20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>256</v>
+      </c>
+      <c r="C21">
+        <v>100</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>7</v>
+      </c>
+      <c r="H21">
+        <v>18</v>
+      </c>
+      <c r="I21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>256</v>
+      </c>
+      <c r="C22">
+        <v>100</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>50</v>
+      </c>
+      <c r="H22">
+        <v>8</v>
+      </c>
+      <c r="I22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>256</v>
+      </c>
+      <c r="C23">
+        <v>100</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>7</v>
+      </c>
+      <c r="H23">
+        <v>48</v>
+      </c>
+      <c r="I23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>256</v>
+      </c>
+      <c r="C24">
+        <v>100</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>50</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>256</v>
+      </c>
+      <c r="C25">
+        <v>100</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>7</v>
+      </c>
+      <c r="H25">
+        <v>9</v>
+      </c>
+      <c r="I25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>512</v>
+      </c>
+      <c r="C26">
+        <v>100</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>50</v>
+      </c>
+      <c r="H26">
+        <v>37</v>
+      </c>
+      <c r="I26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>512</v>
+      </c>
+      <c r="C27">
+        <v>100</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>7</v>
+      </c>
+      <c r="H27">
+        <v>58</v>
+      </c>
+      <c r="I27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>512</v>
+      </c>
+      <c r="C28">
+        <v>100</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>50</v>
+      </c>
+      <c r="H28">
+        <v>26</v>
+      </c>
+      <c r="I28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>512</v>
+      </c>
+      <c r="C29">
+        <v>100</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>7</v>
+      </c>
+      <c r="H29">
+        <v>25</v>
+      </c>
+      <c r="I29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>512</v>
+      </c>
+      <c r="C30">
+        <v>100</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>50</v>
+      </c>
+      <c r="H30">
+        <v>7</v>
+      </c>
+      <c r="I30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>512</v>
+      </c>
+      <c r="C31">
+        <v>100</v>
+      </c>
+      <c r="D31">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <v>7</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+      <c r="I31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>512</v>
+      </c>
+      <c r="C32">
+        <v>100</v>
+      </c>
+      <c r="D32">
+        <v>8</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <v>50</v>
+      </c>
+      <c r="H32">
+        <v>8</v>
+      </c>
+      <c r="I32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>512</v>
+      </c>
+      <c r="C33">
+        <v>100</v>
+      </c>
+      <c r="D33">
+        <v>8</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33">
+        <v>7</v>
+      </c>
+      <c r="H33">
+        <v>35</v>
+      </c>
+      <c r="I33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>512</v>
+      </c>
+      <c r="C34">
+        <v>100</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <v>50</v>
+      </c>
+      <c r="H34">
+        <v>13</v>
+      </c>
+      <c r="I34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>512</v>
+      </c>
+      <c r="C35">
+        <v>100</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <v>7</v>
+      </c>
+      <c r="H35">
+        <v>23</v>
+      </c>
+      <c r="I35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36">
+        <v>25</v>
+      </c>
+      <c r="B36">
+        <v>512</v>
+      </c>
+      <c r="C36">
+        <v>100</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <v>50</v>
+      </c>
+      <c r="H36">
+        <v>39</v>
+      </c>
+      <c r="I36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37">
+        <v>26</v>
+      </c>
+      <c r="B37">
+        <v>512</v>
+      </c>
+      <c r="C37">
+        <v>100</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="F37">
+        <v>7</v>
+      </c>
+      <c r="H37">
+        <v>48</v>
+      </c>
+      <c r="I37" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>